<commit_message>
gnatt chart edit, and images added
</commit_message>
<xml_diff>
--- a/GANTT_Chart.xlsx
+++ b/GANTT_Chart.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/christofer/Desktop/4th Year/PH551/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lewis\Desktop\Education\Uni\PH551_Group_Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC3BCBD9-E2C1-FC41-9491-3719F3AA25A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFA96B4E-62F7-4B56-8C7E-2C01B35D1420}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16500" xr2:uid="{B5873C7A-60BB-0246-BA54-B6C81AEE7422}"/>
+    <workbookView xWindow="12780" yWindow="660" windowWidth="28320" windowHeight="16440" xr2:uid="{B5873C7A-60BB-0246-BA54-B6C81AEE7422}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -23,9 +23,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
@@ -49,9 +47,6 @@
   </si>
   <si>
     <t>Numerical Simulations of Atomic Ensembles in Optical Tweezers</t>
-  </si>
-  <si>
-    <t>Start Building the Experimental Optical Set-Up</t>
   </si>
   <si>
     <t>Run Experiments and Analysis of Data</t>
@@ -123,6 +118,9 @@
   </si>
   <si>
     <t>Budget: £ 384,727.00</t>
+  </si>
+  <si>
+    <t>Building the Experimental Optical Set-Up</t>
   </si>
 </sst>
 </file>
@@ -240,7 +238,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -385,11 +383,29 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
@@ -447,9 +463,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -458,22 +471,29 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -788,30 +808,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6CCEA0E-6C65-AC4D-8706-69E6D21B349B}">
-  <dimension ref="A1:T45"/>
+  <dimension ref="A1:R45"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="108" zoomScaleSheetLayoutView="137" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A2" sqref="A2:J22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="92.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.83203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.1640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.1640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.83203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.1640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.6640625" customWidth="1"/>
-    <col min="11" max="12" width="13.1640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.83203125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="15.1640625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="92.69921875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.19921875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.19921875" customWidth="1"/>
+    <col min="4" max="4" width="13.296875" customWidth="1"/>
+    <col min="5" max="7" width="13.19921875" customWidth="1"/>
+    <col min="8" max="8" width="13.296875" customWidth="1"/>
+    <col min="9" max="10" width="13.19921875" customWidth="1"/>
+    <col min="11" max="11" width="13.796875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.19921875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.69921875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="34" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:18" ht="33.6" x14ac:dyDescent="0.65">
       <c r="B1" s="39" t="s">
         <v>0</v>
       </c>
@@ -823,79 +840,85 @@
       <c r="H1" s="39"/>
       <c r="I1" s="39"/>
       <c r="J1" s="39"/>
-      <c r="K1" s="39"/>
-      <c r="L1" s="39"/>
-      <c r="M1" s="25"/>
-      <c r="N1" s="25"/>
-    </row>
-    <row r="2" spans="1:20" ht="21" x14ac:dyDescent="0.2">
+      <c r="K1" s="25"/>
+      <c r="L1" s="25"/>
+    </row>
+    <row r="2" spans="1:18" ht="21" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="3" spans="1:20" ht="21" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+      <c r="B2" s="41"/>
+      <c r="C2" s="41"/>
+      <c r="D2" s="41"/>
+      <c r="E2" s="41"/>
+      <c r="F2" s="41"/>
+      <c r="G2" s="41"/>
+      <c r="H2" s="41"/>
+      <c r="I2" s="41"/>
+      <c r="J2" s="41"/>
+    </row>
+    <row r="3" spans="1:18" ht="21" x14ac:dyDescent="0.4">
       <c r="A3" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="C3" s="40"/>
-      <c r="D3" s="40"/>
-      <c r="E3" s="40"/>
-      <c r="F3" s="40"/>
-      <c r="G3" s="40"/>
-      <c r="H3" s="40"/>
-      <c r="I3" s="40"/>
-      <c r="J3" s="40"/>
+        <v>21</v>
+      </c>
+      <c r="B3" s="41"/>
+      <c r="C3" s="41"/>
+      <c r="D3" s="41"/>
+      <c r="E3" s="41"/>
+      <c r="F3" s="41"/>
+      <c r="G3" s="41"/>
+      <c r="H3" s="41"/>
+      <c r="I3" s="41"/>
+      <c r="J3" s="41"/>
       <c r="K3" s="40"/>
       <c r="L3" s="40"/>
-      <c r="M3" s="40"/>
-      <c r="N3" s="40"/>
-      <c r="P3" s="24"/>
-    </row>
-    <row r="4" spans="1:20" ht="21" x14ac:dyDescent="0.25">
-      <c r="A4" s="30" t="s">
-        <v>1</v>
-      </c>
-      <c r="B4" s="24"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
-      <c r="H4" s="1"/>
-      <c r="I4" s="1"/>
-      <c r="J4" s="1"/>
+      <c r="N3" s="24"/>
+    </row>
+    <row r="4" spans="1:18" ht="21" x14ac:dyDescent="0.4">
+      <c r="A4" s="30"/>
+      <c r="B4" s="42"/>
+      <c r="C4" s="42"/>
+      <c r="D4" s="42"/>
+      <c r="E4" s="42"/>
+      <c r="F4" s="42"/>
+      <c r="G4" s="42"/>
+      <c r="H4" s="42"/>
+      <c r="I4" s="42"/>
+      <c r="J4" s="42"/>
       <c r="K4" s="1"/>
       <c r="L4" s="1"/>
-      <c r="M4" s="1"/>
-      <c r="N4" s="1"/>
-      <c r="P4" s="24"/>
-    </row>
-    <row r="5" spans="1:20" ht="21" x14ac:dyDescent="0.25">
+      <c r="N4" s="24"/>
+    </row>
+    <row r="5" spans="1:18" ht="21" x14ac:dyDescent="0.4">
+      <c r="A5" s="43" t="s">
+        <v>1</v>
+      </c>
       <c r="B5" s="6">
         <v>2022</v>
       </c>
-      <c r="C5" s="31"/>
-      <c r="D5" s="36">
+      <c r="C5" s="36">
         <v>2023</v>
       </c>
-      <c r="E5" s="38"/>
+      <c r="D5" s="37"/>
+      <c r="E5" s="37"/>
       <c r="F5" s="38"/>
-      <c r="G5" s="37"/>
-      <c r="I5" s="36">
+      <c r="G5" s="36">
         <v>2024</v>
       </c>
+      <c r="H5" s="37"/>
+      <c r="I5" s="37"/>
       <c r="J5" s="38"/>
-      <c r="K5" s="38"/>
-      <c r="L5" s="37"/>
-      <c r="S5" s="41"/>
-      <c r="T5" s="41"/>
-    </row>
-    <row r="6" spans="1:20" ht="21" x14ac:dyDescent="0.2">
-      <c r="A6" s="24"/>
+      <c r="Q5" s="35"/>
+      <c r="R5" s="35"/>
+    </row>
+    <row r="6" spans="1:18" ht="21" x14ac:dyDescent="0.3">
+      <c r="A6" s="43"/>
       <c r="B6" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="C6" s="9"/>
+        <v>18</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>13</v>
+      </c>
       <c r="D6" s="6" t="s">
         <v>14</v>
       </c>
@@ -903,320 +926,295 @@
         <v>15</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="G6" s="6" t="s">
-        <v>19</v>
+        <v>13</v>
+      </c>
+      <c r="H6" s="6" t="s">
+        <v>14</v>
       </c>
       <c r="I6" s="6" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="J6" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="K6" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="L6" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="S6" s="9"/>
-      <c r="T6" s="9"/>
-    </row>
-    <row r="7" spans="1:20" ht="21" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+      <c r="Q6" s="9"/>
+      <c r="R6" s="9"/>
+    </row>
+    <row r="7" spans="1:18" ht="21" x14ac:dyDescent="0.4">
       <c r="A7" s="3"/>
       <c r="B7" s="13"/>
-      <c r="C7" s="14"/>
+      <c r="C7" s="13"/>
       <c r="D7" s="13"/>
       <c r="E7" s="13"/>
       <c r="F7" s="13"/>
       <c r="G7" s="13"/>
+      <c r="H7" s="13"/>
       <c r="I7" s="13"/>
       <c r="J7" s="13"/>
-      <c r="K7" s="13"/>
-      <c r="L7" s="13"/>
-      <c r="S7" s="16"/>
-      <c r="T7" s="16"/>
-    </row>
-    <row r="8" spans="1:20" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Q7" s="16"/>
+      <c r="R7" s="16"/>
+    </row>
+    <row r="8" spans="1:18" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A8" s="8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
       <c r="I8" s="1"/>
-      <c r="J8" s="1"/>
-      <c r="K8" s="1"/>
-      <c r="S8" s="16"/>
-      <c r="T8" s="16"/>
-    </row>
-    <row r="9" spans="1:20" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Q8" s="16"/>
+      <c r="R8" s="16"/>
+    </row>
+    <row r="9" spans="1:18" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A9" s="28" t="s">
         <v>2</v>
       </c>
       <c r="B9" s="15"/>
-      <c r="C9" s="2"/>
+      <c r="C9" s="1"/>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
       <c r="I9" s="1"/>
-      <c r="J9" s="1"/>
-      <c r="K9" s="1"/>
-      <c r="S9" s="16"/>
-      <c r="T9" s="16"/>
-    </row>
-    <row r="10" spans="1:20" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="33" t="s">
+      <c r="Q9" s="16"/>
+      <c r="R9" s="16"/>
+    </row>
+    <row r="10" spans="1:18" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A10" s="32" t="s">
         <v>3</v>
       </c>
       <c r="B10" s="26"/>
-      <c r="C10" s="16"/>
-      <c r="D10" s="19"/>
+      <c r="C10" s="19"/>
+      <c r="D10" s="1"/>
       <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
       <c r="I10" s="1"/>
-      <c r="J10" s="1"/>
-      <c r="K10" s="1"/>
-      <c r="S10" s="16"/>
-      <c r="T10" s="16"/>
-    </row>
-    <row r="11" spans="1:20" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Q10" s="16"/>
+      <c r="R10" s="16"/>
+    </row>
+    <row r="11" spans="1:18" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A11" s="27" t="s">
         <v>4</v>
       </c>
       <c r="B11" s="15"/>
-      <c r="C11" s="16"/>
-      <c r="D11" s="15"/>
+      <c r="C11" s="15"/>
+      <c r="D11" s="1"/>
       <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
       <c r="I11" s="1"/>
-      <c r="J11" s="1"/>
-      <c r="K11" s="1"/>
-      <c r="S11" s="16"/>
-      <c r="T11" s="16"/>
-    </row>
-    <row r="12" spans="1:20" s="4" customFormat="1" ht="21" x14ac:dyDescent="0.25">
+      <c r="Q11" s="16"/>
+      <c r="R11" s="16"/>
+    </row>
+    <row r="12" spans="1:18" s="4" customFormat="1" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A12" s="7" t="s">
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="B12" s="14"/>
-      <c r="C12" s="16"/>
-      <c r="D12" s="16"/>
+      <c r="C12" s="15"/>
+      <c r="D12" s="15"/>
       <c r="E12" s="16"/>
-      <c r="F12" s="16"/>
+      <c r="G12" s="14"/>
+      <c r="H12" s="14"/>
       <c r="I12" s="14"/>
-      <c r="J12" s="14"/>
-      <c r="K12" s="14"/>
-      <c r="S12" s="16"/>
-      <c r="T12" s="16"/>
-    </row>
-    <row r="13" spans="1:20" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Q12" s="16"/>
+      <c r="R12" s="16"/>
+    </row>
+    <row r="13" spans="1:18" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A13" s="10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
+      <c r="D13" s="16"/>
       <c r="E13" s="16"/>
-      <c r="F13" s="16"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1"/>
       <c r="I13" s="1"/>
-      <c r="J13" s="1"/>
-      <c r="K13" s="1"/>
-      <c r="S13" s="16"/>
-      <c r="T13" s="16"/>
-    </row>
-    <row r="14" spans="1:20" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Q13" s="16"/>
+      <c r="R13" s="16"/>
+    </row>
+    <row r="14" spans="1:18" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A14" s="7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
-      <c r="D14" s="17"/>
-      <c r="E14" s="20"/>
-      <c r="F14" s="16"/>
+      <c r="D14" s="20"/>
+      <c r="E14" s="17"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1"/>
       <c r="I14" s="1"/>
-      <c r="J14" s="1"/>
-      <c r="K14" s="1"/>
-      <c r="S14" s="16"/>
-      <c r="T14" s="16"/>
-    </row>
-    <row r="15" spans="1:20" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Q14" s="16"/>
+      <c r="R14" s="16"/>
+    </row>
+    <row r="15" spans="1:18" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A15" s="9" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
-      <c r="F15" s="34"/>
+      <c r="E15" s="33"/>
+      <c r="F15" s="33"/>
+      <c r="G15" s="1"/>
+      <c r="H15" s="1"/>
       <c r="I15" s="1"/>
-      <c r="J15" s="1"/>
-      <c r="K15" s="1"/>
-      <c r="S15" s="16"/>
-      <c r="T15" s="16"/>
-    </row>
-    <row r="16" spans="1:20" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Q15" s="16"/>
+      <c r="R15" s="16"/>
+    </row>
+    <row r="16" spans="1:18" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A16" s="11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
-      <c r="E16" s="1"/>
       <c r="F16" s="17"/>
-      <c r="G16" s="24"/>
+      <c r="G16" s="1"/>
+      <c r="H16" s="1"/>
       <c r="I16" s="1"/>
-      <c r="J16" s="1"/>
-      <c r="K16" s="1"/>
-      <c r="S16" s="16"/>
-      <c r="T16" s="16"/>
-    </row>
-    <row r="17" spans="1:20" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Q16" s="16"/>
+      <c r="R16" s="16"/>
+    </row>
+    <row r="17" spans="1:18" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A17" s="21" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B17" s="14"/>
       <c r="C17" s="14"/>
-      <c r="D17" s="14"/>
-      <c r="E17" s="16"/>
+      <c r="D17" s="16"/>
+      <c r="E17" s="14"/>
       <c r="F17" s="14"/>
       <c r="G17" s="14"/>
+      <c r="H17" s="14"/>
       <c r="I17" s="14"/>
-      <c r="J17" s="14"/>
-      <c r="K17" s="14"/>
-      <c r="S17" s="16"/>
-      <c r="T17" s="16"/>
-    </row>
-    <row r="18" spans="1:20" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Q17" s="16"/>
+      <c r="R17" s="16"/>
+    </row>
+    <row r="18" spans="1:18" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A18" s="12" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
-      <c r="D18" s="1"/>
-      <c r="E18" s="16"/>
+      <c r="D18" s="16"/>
+      <c r="E18" s="1"/>
       <c r="F18" s="1"/>
-      <c r="G18" s="1"/>
+      <c r="G18" s="18"/>
+      <c r="H18" s="18"/>
       <c r="I18" s="18"/>
       <c r="J18" s="18"/>
-      <c r="K18" s="18"/>
-      <c r="L18" s="18"/>
-      <c r="S18" s="16"/>
-      <c r="T18" s="16"/>
-    </row>
-    <row r="19" spans="1:20" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Q18" s="16"/>
+      <c r="R18" s="16"/>
+    </row>
+    <row r="19" spans="1:18" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A19" s="12" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B19" s="14"/>
       <c r="C19" s="14"/>
-      <c r="D19" s="14"/>
-      <c r="E19" s="16"/>
+      <c r="D19" s="16"/>
+      <c r="E19" s="14"/>
       <c r="F19" s="14"/>
-      <c r="G19" s="14"/>
-      <c r="I19" s="35"/>
-      <c r="J19" s="16"/>
-      <c r="S19" s="16"/>
-      <c r="T19" s="16"/>
-    </row>
-    <row r="20" spans="1:20" s="4" customFormat="1" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G19" s="34"/>
+      <c r="H19" s="16"/>
+      <c r="Q19" s="16"/>
+      <c r="R19" s="16"/>
+    </row>
+    <row r="20" spans="1:18" s="4" customFormat="1" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A20" s="11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B20" s="14"/>
       <c r="C20" s="14"/>
-      <c r="D20" s="14"/>
-      <c r="E20" s="16"/>
+      <c r="D20" s="16"/>
+      <c r="E20" s="14"/>
       <c r="F20" s="14"/>
-      <c r="G20" s="14"/>
-      <c r="I20" s="16"/>
-      <c r="J20" s="16"/>
-      <c r="K20" s="35"/>
-      <c r="T20" s="16"/>
-    </row>
-    <row r="21" spans="1:20" s="4" customFormat="1" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G20" s="16"/>
+      <c r="H20" s="16"/>
+      <c r="I20" s="34"/>
+      <c r="R20" s="16"/>
+    </row>
+    <row r="21" spans="1:18" s="4" customFormat="1" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A21" s="11" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B21" s="14"/>
       <c r="C21" s="14"/>
-      <c r="D21" s="14"/>
-      <c r="E21" s="16"/>
+      <c r="D21" s="16"/>
+      <c r="E21" s="14"/>
       <c r="F21" s="14"/>
-      <c r="G21" s="14"/>
+      <c r="G21" s="16"/>
       <c r="H21" s="16"/>
-      <c r="I21" s="16"/>
-      <c r="J21" s="16"/>
-      <c r="K21" s="29"/>
-      <c r="L21" s="18"/>
-      <c r="P21" s="16"/>
-      <c r="S21" s="16"/>
-    </row>
-    <row r="22" spans="1:20" s="4" customFormat="1" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I21" s="29"/>
+      <c r="J21" s="18"/>
+      <c r="N21" s="16"/>
+      <c r="Q21" s="16"/>
+    </row>
+    <row r="22" spans="1:18" s="4" customFormat="1" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A22" s="11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B22" s="14"/>
       <c r="C22" s="14"/>
-      <c r="D22" s="14"/>
-      <c r="E22" s="16"/>
+      <c r="D22" s="16"/>
+      <c r="E22" s="14"/>
       <c r="F22" s="14"/>
-      <c r="G22" s="14"/>
+      <c r="G22" s="16"/>
       <c r="H22" s="16"/>
-      <c r="I22" s="16"/>
-      <c r="J22" s="16"/>
-      <c r="K22" s="29"/>
-      <c r="L22" s="18"/>
-      <c r="P22" s="16"/>
-      <c r="S22" s="16"/>
-    </row>
-    <row r="24" spans="1:20" s="4" customFormat="1" ht="21" x14ac:dyDescent="0.25">
-      <c r="P24" s="16"/>
-    </row>
-    <row r="25" spans="1:20" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="P25" s="29"/>
-    </row>
-    <row r="26" spans="1:20" ht="21" x14ac:dyDescent="0.25">
+      <c r="I22" s="29"/>
+      <c r="J22" s="18"/>
+      <c r="N22" s="16"/>
+      <c r="Q22" s="16"/>
+    </row>
+    <row r="24" spans="1:18" s="4" customFormat="1" ht="21" x14ac:dyDescent="0.4">
+      <c r="N24" s="16"/>
+    </row>
+    <row r="25" spans="1:18" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="N25" s="29"/>
+    </row>
+    <row r="26" spans="1:18" ht="21" x14ac:dyDescent="0.4">
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
-      <c r="D26" s="1"/>
-      <c r="E26" s="16"/>
+      <c r="D26" s="16"/>
+      <c r="E26" s="1"/>
       <c r="F26" s="1"/>
       <c r="G26" s="1"/>
       <c r="H26" s="1"/>
       <c r="I26" s="1"/>
       <c r="J26" s="1"/>
-      <c r="K26" s="1"/>
-      <c r="L26" s="1"/>
-      <c r="M26" s="2"/>
-      <c r="N26" s="23"/>
-      <c r="O26" s="16"/>
-      <c r="P26" s="24"/>
-    </row>
-    <row r="27" spans="1:20" ht="21" x14ac:dyDescent="0.25">
+      <c r="K26" s="2"/>
+      <c r="L26" s="23"/>
+      <c r="M26" s="16"/>
+      <c r="N26" s="24"/>
+    </row>
+    <row r="27" spans="1:18" ht="21" x14ac:dyDescent="0.4">
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
-      <c r="D27" s="1"/>
-      <c r="E27" s="16"/>
+      <c r="D27" s="16"/>
+      <c r="E27" s="1"/>
       <c r="F27" s="1"/>
       <c r="G27" s="1"/>
-      <c r="H27" s="1"/>
+      <c r="H27" s="22"/>
       <c r="I27" s="1"/>
-      <c r="J27" s="22"/>
+      <c r="J27" s="1"/>
       <c r="K27" s="1"/>
       <c r="L27" s="1"/>
-      <c r="M27" s="1"/>
-      <c r="N27" s="1"/>
-      <c r="O27" s="16"/>
-    </row>
-    <row r="28" spans="1:20" ht="21" x14ac:dyDescent="0.25">
+      <c r="M27" s="16"/>
+    </row>
+    <row r="28" spans="1:18" ht="21" x14ac:dyDescent="0.4">
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
-      <c r="D28" s="1"/>
-      <c r="E28" s="16"/>
+      <c r="D28" s="16"/>
+      <c r="E28" s="1"/>
       <c r="F28" s="1"/>
       <c r="G28" s="1"/>
       <c r="H28" s="1"/>
@@ -1225,121 +1223,106 @@
       <c r="K28" s="1"/>
       <c r="L28" s="1"/>
       <c r="M28" s="1"/>
-      <c r="N28" s="1"/>
-      <c r="O28" s="1"/>
-    </row>
-    <row r="29" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="O29" s="24"/>
-    </row>
-    <row r="32" spans="1:20" x14ac:dyDescent="0.2">
+    </row>
+    <row r="29" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="M29" s="24"/>
+    </row>
+    <row r="32" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A32" s="29"/>
       <c r="B32" s="29"/>
       <c r="C32" s="29"/>
       <c r="D32" s="29"/>
-      <c r="E32" s="29"/>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" s="29"/>
       <c r="B33" s="29"/>
       <c r="C33" s="29"/>
       <c r="D33" s="29"/>
-      <c r="E33" s="29"/>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" s="29"/>
       <c r="B34" s="29"/>
       <c r="C34" s="29"/>
       <c r="D34" s="29"/>
-      <c r="E34" s="29"/>
-    </row>
-    <row r="35" spans="1:5" ht="21" x14ac:dyDescent="0.2">
+    </row>
+    <row r="35" spans="1:4" ht="21" x14ac:dyDescent="0.3">
       <c r="A35" s="29"/>
-      <c r="B35" s="32"/>
-      <c r="C35" s="32"/>
-      <c r="D35" s="32"/>
-      <c r="E35" s="29"/>
-    </row>
-    <row r="36" spans="1:5" ht="21" x14ac:dyDescent="0.2">
+      <c r="B35" s="31"/>
+      <c r="C35" s="31"/>
+      <c r="D35" s="29"/>
+    </row>
+    <row r="36" spans="1:4" ht="21" x14ac:dyDescent="0.3">
       <c r="A36" s="29"/>
       <c r="B36" s="9"/>
       <c r="C36" s="9"/>
-      <c r="D36" s="9"/>
-      <c r="E36" s="29"/>
-    </row>
-    <row r="37" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+      <c r="D36" s="29"/>
+    </row>
+    <row r="37" spans="1:4" ht="21" x14ac:dyDescent="0.4">
       <c r="A37" s="29"/>
       <c r="B37" s="16"/>
       <c r="C37" s="16"/>
-      <c r="D37" s="16"/>
-      <c r="E37" s="29"/>
-    </row>
-    <row r="38" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+      <c r="D37" s="29"/>
+    </row>
+    <row r="38" spans="1:4" ht="21" x14ac:dyDescent="0.4">
       <c r="A38" s="29"/>
       <c r="B38" s="16"/>
       <c r="C38" s="16"/>
-      <c r="D38" s="16"/>
-      <c r="E38" s="29"/>
-    </row>
-    <row r="39" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+      <c r="D38" s="29"/>
+    </row>
+    <row r="39" spans="1:4" ht="21" x14ac:dyDescent="0.4">
       <c r="A39" s="29"/>
       <c r="B39" s="16"/>
       <c r="C39" s="16"/>
-      <c r="D39" s="16"/>
-      <c r="E39" s="29"/>
-    </row>
-    <row r="40" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+      <c r="D39" s="29"/>
+    </row>
+    <row r="40" spans="1:4" ht="21" x14ac:dyDescent="0.4">
       <c r="A40" s="29"/>
       <c r="B40" s="16"/>
       <c r="C40" s="16"/>
-      <c r="D40" s="16"/>
-      <c r="E40" s="29"/>
-    </row>
-    <row r="41" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+      <c r="D40" s="29"/>
+    </row>
+    <row r="41" spans="1:4" ht="21" x14ac:dyDescent="0.4">
       <c r="A41" s="29"/>
       <c r="B41" s="16"/>
       <c r="C41" s="16"/>
-      <c r="D41" s="16"/>
-      <c r="E41" s="29"/>
-    </row>
-    <row r="42" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+      <c r="D41" s="29"/>
+    </row>
+    <row r="42" spans="1:4" ht="21" x14ac:dyDescent="0.4">
       <c r="A42" s="29"/>
       <c r="B42" s="16"/>
       <c r="C42" s="16"/>
-      <c r="D42" s="16"/>
-      <c r="E42" s="29"/>
-    </row>
-    <row r="43" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+      <c r="D42" s="29"/>
+    </row>
+    <row r="43" spans="1:4" ht="21" x14ac:dyDescent="0.4">
       <c r="A43" s="29"/>
       <c r="B43" s="16"/>
       <c r="C43" s="16"/>
-      <c r="D43" s="16"/>
-      <c r="E43" s="29"/>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D43" s="29"/>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44" s="29"/>
       <c r="B44" s="29"/>
       <c r="C44" s="29"/>
       <c r="D44" s="29"/>
-      <c r="E44" s="29"/>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45" s="29"/>
       <c r="B45" s="29"/>
       <c r="C45" s="29"/>
       <c r="D45" s="29"/>
-      <c r="E45" s="29"/>
     </row>
   </sheetData>
-  <mergeCells count="6">
-    <mergeCell ref="C3:F3"/>
-    <mergeCell ref="G3:J3"/>
-    <mergeCell ref="K3:N3"/>
-    <mergeCell ref="D5:G5"/>
-    <mergeCell ref="I5:L5"/>
-    <mergeCell ref="B1:L1"/>
+  <mergeCells count="7">
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="B1:J1"/>
+    <mergeCell ref="C2:F4"/>
+    <mergeCell ref="G2:J4"/>
+    <mergeCell ref="B2:B4"/>
+    <mergeCell ref="C5:F5"/>
+    <mergeCell ref="G5:J5"/>
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
images added and updated gantt
</commit_message>
<xml_diff>
--- a/GANTT_Chart.xlsx
+++ b/GANTT_Chart.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/christofer/Desktop/4th Year/PH551/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lewis\Desktop\Education\Uni\PH551_Group_Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1676B5D-F313-6E4B-8988-AD952AE1F4A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58EE6CDC-253E-4923-A13B-090140DDB35F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16500" xr2:uid="{B5873C7A-60BB-0246-BA54-B6C81AEE7422}"/>
+    <workbookView xWindow="12768" yWindow="672" windowWidth="28320" windowHeight="16464" xr2:uid="{B5873C7A-60BB-0246-BA54-B6C81AEE7422}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -23,9 +23,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
@@ -48,9 +46,6 @@
     <t>Numerical Simulations of Atomic Ensembles in Optical Tweezers</t>
   </si>
   <si>
-    <t>Start Building the Experimental Optical Set-Up</t>
-  </si>
-  <si>
     <t>Run Experiments and Analysis of Data</t>
   </si>
   <si>
@@ -85,29 +80,6 @@
   </si>
   <si>
     <t>Organise: Workshop in Advances in Quantum Hardware (WAQC '24): Beijing, China</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="18"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Proposed Starting Point:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="18"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> Monday 1st of September 2022 </t>
-    </r>
   </si>
   <si>
     <r>
@@ -172,6 +144,32 @@
         <family val="2"/>
       </rPr>
       <t>Outreach and Industrial R&amp;D</t>
+    </r>
+  </si>
+  <si>
+    <t>Building the Experimental Optical Set-Up</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="18"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Proposed Starting Date:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Monday 1st of September 2022 </t>
     </r>
   </si>
 </sst>
@@ -540,7 +538,19 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -555,19 +565,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -887,67 +885,67 @@
   <dimension ref="A1:T45"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="108" zoomScaleSheetLayoutView="137" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+      <selection activeCell="K3" sqref="K3:N3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="92.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.83203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.1640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.1640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.83203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.1640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.6640625" customWidth="1"/>
-    <col min="11" max="12" width="13.1640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.83203125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="15.1640625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="92.69921875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.19921875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.19921875" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="14.69921875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.19921875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.796875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.19921875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.69921875" customWidth="1"/>
+    <col min="11" max="12" width="13.19921875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.796875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15.19921875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="14.69921875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="34" x14ac:dyDescent="0.4">
-      <c r="B1" s="36" t="s">
+    <row r="1" spans="1:20" ht="33.6" x14ac:dyDescent="0.65">
+      <c r="B1" s="40" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="36"/>
-      <c r="D1" s="36"/>
-      <c r="E1" s="36"/>
-      <c r="F1" s="36"/>
-      <c r="G1" s="36"/>
-      <c r="H1" s="36"/>
-      <c r="I1" s="36"/>
-      <c r="J1" s="36"/>
+      <c r="C1" s="40"/>
+      <c r="D1" s="40"/>
+      <c r="E1" s="40"/>
+      <c r="F1" s="40"/>
+      <c r="G1" s="40"/>
+      <c r="H1" s="40"/>
+      <c r="I1" s="40"/>
+      <c r="J1" s="40"/>
       <c r="K1" s="21"/>
       <c r="L1" s="21"/>
       <c r="M1" s="21"/>
       <c r="N1" s="21"/>
     </row>
-    <row r="2" spans="1:20" ht="24" x14ac:dyDescent="0.2">
-      <c r="A2" s="40" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="3" spans="1:20" ht="24" x14ac:dyDescent="0.3">
-      <c r="A3" s="41" t="s">
-        <v>18</v>
-      </c>
-      <c r="C3" s="32"/>
-      <c r="D3" s="32"/>
-      <c r="E3" s="32"/>
-      <c r="F3" s="32"/>
-      <c r="G3" s="32"/>
-      <c r="H3" s="32"/>
-      <c r="I3" s="32"/>
-      <c r="J3" s="32"/>
-      <c r="K3" s="32"/>
-      <c r="L3" s="32"/>
-      <c r="M3" s="32"/>
-      <c r="N3" s="32"/>
+    <row r="2" spans="1:20" ht="23.4" x14ac:dyDescent="0.3">
+      <c r="A2" s="35" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="A3" s="36" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" s="41"/>
+      <c r="D3" s="41"/>
+      <c r="E3" s="41"/>
+      <c r="F3" s="41"/>
+      <c r="G3" s="41"/>
+      <c r="H3" s="41"/>
+      <c r="I3" s="41"/>
+      <c r="J3" s="41"/>
+      <c r="K3" s="41"/>
+      <c r="L3" s="41"/>
+      <c r="M3" s="41"/>
+      <c r="N3" s="41"/>
       <c r="P3" s="20"/>
     </row>
-    <row r="4" spans="1:20" ht="21" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:20" ht="21" x14ac:dyDescent="0.4">
       <c r="A4" s="26"/>
       <c r="B4" s="20"/>
       <c r="C4" s="2"/>
@@ -964,58 +962,58 @@
       <c r="N4" s="1"/>
       <c r="P4" s="20"/>
     </row>
-    <row r="5" spans="1:20" ht="21" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:20" ht="21" x14ac:dyDescent="0.4">
       <c r="B5" s="5">
         <v>2022</v>
       </c>
-      <c r="C5" s="33">
+      <c r="C5" s="37">
         <v>2023</v>
       </c>
-      <c r="D5" s="34"/>
-      <c r="E5" s="34"/>
-      <c r="F5" s="35"/>
-      <c r="G5" s="33">
+      <c r="D5" s="38"/>
+      <c r="E5" s="38"/>
+      <c r="F5" s="39"/>
+      <c r="G5" s="37">
         <v>2024</v>
       </c>
-      <c r="H5" s="34"/>
-      <c r="I5" s="34"/>
-      <c r="J5" s="35"/>
+      <c r="H5" s="38"/>
+      <c r="I5" s="38"/>
+      <c r="J5" s="39"/>
       <c r="S5" s="31"/>
       <c r="T5" s="31"/>
     </row>
-    <row r="6" spans="1:20" ht="21" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:20" ht="21" x14ac:dyDescent="0.3">
       <c r="A6" s="20"/>
       <c r="B6" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C6" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="D6" s="5" t="s">
+      <c r="E6" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E6" s="5" t="s">
-        <v>12</v>
-      </c>
       <c r="F6" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G6" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="H6" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="H6" s="5" t="s">
+      <c r="I6" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="I6" s="5" t="s">
-        <v>12</v>
-      </c>
       <c r="J6" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="S6" s="7"/>
       <c r="T6" s="7"/>
     </row>
-    <row r="7" spans="1:20" ht="21" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:20" ht="21" x14ac:dyDescent="0.4">
       <c r="A7" s="3"/>
       <c r="B7" s="10"/>
       <c r="C7" s="10"/>
@@ -1029,9 +1027,9 @@
       <c r="S7" s="13"/>
       <c r="T7" s="13"/>
     </row>
-    <row r="8" spans="1:20" ht="24" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="37" t="s">
-        <v>19</v>
+    <row r="8" spans="1:20" ht="23.4" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A8" s="32" t="s">
+        <v>17</v>
       </c>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
@@ -1043,7 +1041,7 @@
       <c r="S8" s="13"/>
       <c r="T8" s="13"/>
     </row>
-    <row r="9" spans="1:20" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:20" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A9" s="24" t="s">
         <v>1</v>
       </c>
@@ -1057,7 +1055,7 @@
       <c r="S9" s="13"/>
       <c r="T9" s="13"/>
     </row>
-    <row r="10" spans="1:20" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:20" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A10" s="28" t="s">
         <v>2</v>
       </c>
@@ -1071,7 +1069,7 @@
       <c r="S10" s="13"/>
       <c r="T10" s="13"/>
     </row>
-    <row r="11" spans="1:20" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:20" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A11" s="23" t="s">
         <v>3</v>
       </c>
@@ -1085,13 +1083,13 @@
       <c r="S11" s="13"/>
       <c r="T11" s="13"/>
     </row>
-    <row r="12" spans="1:20" s="4" customFormat="1" ht="21" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:20" s="4" customFormat="1" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A12" s="6" t="s">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="B12" s="11"/>
-      <c r="C12" s="13"/>
-      <c r="D12" s="13"/>
+      <c r="C12" s="12"/>
+      <c r="D12" s="12"/>
       <c r="E12" s="13"/>
       <c r="G12" s="11"/>
       <c r="H12" s="11"/>
@@ -1099,9 +1097,9 @@
       <c r="S12" s="13"/>
       <c r="T12" s="13"/>
     </row>
-    <row r="13" spans="1:20" ht="26" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="38" t="s">
-        <v>20</v>
+    <row r="13" spans="1:20" ht="25.2" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A13" s="33" t="s">
+        <v>18</v>
       </c>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
@@ -1113,52 +1111,53 @@
       <c r="S13" s="13"/>
       <c r="T13" s="13"/>
     </row>
-    <row r="14" spans="1:20" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:20" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A14" s="6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B14" s="1"/>
-      <c r="C14" s="14"/>
+      <c r="C14" s="1"/>
       <c r="D14" s="17"/>
-      <c r="E14" s="13"/>
+      <c r="E14" s="14"/>
       <c r="G14" s="1"/>
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
       <c r="S14" s="13"/>
       <c r="T14" s="13"/>
     </row>
-    <row r="15" spans="1:20" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:20" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A15" s="7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
       <c r="E15" s="29"/>
+      <c r="F15" s="14"/>
       <c r="G15" s="1"/>
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
       <c r="S15" s="13"/>
       <c r="T15" s="13"/>
     </row>
-    <row r="16" spans="1:20" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:20" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A16" s="8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
-      <c r="E16" s="14"/>
-      <c r="F16" s="20"/>
+      <c r="E16" s="13"/>
+      <c r="F16" s="14"/>
       <c r="G16" s="1"/>
       <c r="H16" s="1"/>
       <c r="I16" s="1"/>
       <c r="S16" s="13"/>
       <c r="T16" s="13"/>
     </row>
-    <row r="17" spans="1:20" ht="26" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="39" t="s">
-        <v>21</v>
+    <row r="17" spans="1:20" ht="25.2" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A17" s="34" t="s">
+        <v>19</v>
       </c>
       <c r="B17" s="11"/>
       <c r="C17" s="11"/>
@@ -1171,9 +1170,9 @@
       <c r="S17" s="13"/>
       <c r="T17" s="13"/>
     </row>
-    <row r="18" spans="1:20" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:20" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A18" s="9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
@@ -1187,9 +1186,9 @@
       <c r="S18" s="13"/>
       <c r="T18" s="13"/>
     </row>
-    <row r="19" spans="1:20" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:20" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A19" s="9" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B19" s="11"/>
       <c r="C19" s="11"/>
@@ -1201,9 +1200,9 @@
       <c r="S19" s="13"/>
       <c r="T19" s="13"/>
     </row>
-    <row r="20" spans="1:20" s="4" customFormat="1" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:20" s="4" customFormat="1" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A20" s="8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B20" s="11"/>
       <c r="C20" s="11"/>
@@ -1215,9 +1214,9 @@
       <c r="I20" s="30"/>
       <c r="T20" s="13"/>
     </row>
-    <row r="21" spans="1:20" s="4" customFormat="1" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:20" s="4" customFormat="1" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A21" s="8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B21" s="11"/>
       <c r="C21" s="11"/>
@@ -1231,9 +1230,9 @@
       <c r="P21" s="13"/>
       <c r="S21" s="13"/>
     </row>
-    <row r="22" spans="1:20" s="4" customFormat="1" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:20" s="4" customFormat="1" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A22" s="8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B22" s="11"/>
       <c r="C22" s="11"/>
@@ -1247,13 +1246,13 @@
       <c r="P22" s="13"/>
       <c r="S22" s="13"/>
     </row>
-    <row r="24" spans="1:20" s="4" customFormat="1" ht="21" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:20" s="4" customFormat="1" ht="21" x14ac:dyDescent="0.4">
       <c r="P24" s="13"/>
     </row>
-    <row r="25" spans="1:20" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:20" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="P25" s="25"/>
     </row>
-    <row r="26" spans="1:20" ht="21" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:20" ht="21" x14ac:dyDescent="0.4">
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
       <c r="D26" s="1"/>
@@ -1270,7 +1269,7 @@
       <c r="O26" s="13"/>
       <c r="P26" s="20"/>
     </row>
-    <row r="27" spans="1:20" ht="21" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:20" ht="21" x14ac:dyDescent="0.4">
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
       <c r="D27" s="1"/>
@@ -1286,7 +1285,7 @@
       <c r="N27" s="1"/>
       <c r="O27" s="13"/>
     </row>
-    <row r="28" spans="1:20" ht="21" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:20" ht="21" x14ac:dyDescent="0.4">
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
       <c r="D28" s="1"/>
@@ -1302,101 +1301,101 @@
       <c r="N28" s="1"/>
       <c r="O28" s="1"/>
     </row>
-    <row r="29" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:20" x14ac:dyDescent="0.3">
       <c r="O29" s="20"/>
     </row>
-    <row r="32" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A32" s="25"/>
       <c r="B32" s="25"/>
       <c r="C32" s="25"/>
       <c r="D32" s="25"/>
       <c r="E32" s="25"/>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" s="25"/>
       <c r="B33" s="25"/>
       <c r="C33" s="25"/>
       <c r="D33" s="25"/>
       <c r="E33" s="25"/>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" s="25"/>
       <c r="B34" s="25"/>
       <c r="C34" s="25"/>
       <c r="D34" s="25"/>
       <c r="E34" s="25"/>
     </row>
-    <row r="35" spans="1:5" ht="21" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:5" ht="21" x14ac:dyDescent="0.3">
       <c r="A35" s="25"/>
       <c r="B35" s="27"/>
       <c r="C35" s="27"/>
       <c r="D35" s="27"/>
       <c r="E35" s="25"/>
     </row>
-    <row r="36" spans="1:5" ht="21" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:5" ht="21" x14ac:dyDescent="0.3">
       <c r="A36" s="25"/>
       <c r="B36" s="7"/>
       <c r="C36" s="7"/>
       <c r="D36" s="7"/>
       <c r="E36" s="25"/>
     </row>
-    <row r="37" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" ht="21" x14ac:dyDescent="0.4">
       <c r="A37" s="25"/>
       <c r="B37" s="13"/>
       <c r="C37" s="13"/>
       <c r="D37" s="13"/>
       <c r="E37" s="25"/>
     </row>
-    <row r="38" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" ht="21" x14ac:dyDescent="0.4">
       <c r="A38" s="25"/>
       <c r="B38" s="13"/>
       <c r="C38" s="13"/>
       <c r="D38" s="13"/>
       <c r="E38" s="25"/>
     </row>
-    <row r="39" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" ht="21" x14ac:dyDescent="0.4">
       <c r="A39" s="25"/>
       <c r="B39" s="13"/>
       <c r="C39" s="13"/>
       <c r="D39" s="13"/>
       <c r="E39" s="25"/>
     </row>
-    <row r="40" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" ht="21" x14ac:dyDescent="0.4">
       <c r="A40" s="25"/>
       <c r="B40" s="13"/>
       <c r="C40" s="13"/>
       <c r="D40" s="13"/>
       <c r="E40" s="25"/>
     </row>
-    <row r="41" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" ht="21" x14ac:dyDescent="0.4">
       <c r="A41" s="25"/>
       <c r="B41" s="13"/>
       <c r="C41" s="13"/>
       <c r="D41" s="13"/>
       <c r="E41" s="25"/>
     </row>
-    <row r="42" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" ht="21" x14ac:dyDescent="0.4">
       <c r="A42" s="25"/>
       <c r="B42" s="13"/>
       <c r="C42" s="13"/>
       <c r="D42" s="13"/>
       <c r="E42" s="25"/>
     </row>
-    <row r="43" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" ht="21" x14ac:dyDescent="0.4">
       <c r="A43" s="25"/>
       <c r="B43" s="13"/>
       <c r="C43" s="13"/>
       <c r="D43" s="13"/>
       <c r="E43" s="25"/>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A44" s="25"/>
       <c r="B44" s="25"/>
       <c r="C44" s="25"/>
       <c r="D44" s="25"/>
       <c r="E44" s="25"/>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A45" s="25"/>
       <c r="B45" s="25"/>
       <c r="C45" s="25"/>
@@ -1405,12 +1404,12 @@
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="K3:N3"/>
     <mergeCell ref="C5:F5"/>
     <mergeCell ref="G5:J5"/>
     <mergeCell ref="B1:J1"/>
     <mergeCell ref="C3:F3"/>
     <mergeCell ref="G3:J3"/>
-    <mergeCell ref="K3:N3"/>
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
image updates and src backup
</commit_message>
<xml_diff>
--- a/GANTT_Chart.xlsx
+++ b/GANTT_Chart.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lewis\Desktop\Education\Uni\PH551_Group_Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58EE6CDC-253E-4923-A13B-090140DDB35F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13844185-E8F5-4F6E-9EF9-22EC218F03E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="12768" yWindow="672" windowWidth="28320" windowHeight="16464" xr2:uid="{B5873C7A-60BB-0246-BA54-B6C81AEE7422}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="22">
   <si>
     <t>MITIGATING  JOULE EXPANSION IN MULTI-CELL ATOMIC MEMORY</t>
   </si>
@@ -61,19 +61,7 @@
     <t>Overall Project Valuation</t>
   </si>
   <si>
-    <t>Quarter I</t>
-  </si>
-  <si>
-    <t>Quarter II</t>
-  </si>
-  <si>
-    <t>Quarter III</t>
-  </si>
-  <si>
     <t>Progress Report</t>
-  </si>
-  <si>
-    <t>Quarter IV</t>
   </si>
   <si>
     <t>Organise: Workshop in Advances in Quantum Hardware (WAQC '24): Glasgow, U.K</t>
@@ -172,12 +160,24 @@
       <t xml:space="preserve"> Monday 1st of September 2022 </t>
     </r>
   </si>
+  <si>
+    <t>Q4</t>
+  </si>
+  <si>
+    <t>Q1</t>
+  </si>
+  <si>
+    <t>Q2</t>
+  </si>
+  <si>
+    <t>Q3</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="16" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -194,22 +194,6 @@
     </font>
     <font>
       <sz val="16"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="16"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="14"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -483,13 +467,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -500,10 +481,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -513,9 +494,9 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -526,31 +507,30 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -562,12 +542,11 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -882,537 +861,546 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6CCEA0E-6C65-AC4D-8706-69E6D21B349B}">
-  <dimension ref="A1:T45"/>
+  <dimension ref="A1:T44"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="108" zoomScaleSheetLayoutView="137" workbookViewId="0">
-      <selection activeCell="K3" sqref="K3:N3"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScaleNormal="100" zoomScaleSheetLayoutView="137" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="92.69921875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.19921875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.796875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.19921875" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="14.69921875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.19921875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.796875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.19921875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.69921875" customWidth="1"/>
-    <col min="11" max="12" width="13.19921875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="13" width="10" customWidth="1"/>
     <col min="14" max="14" width="15.19921875" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="14.69921875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="33.6" x14ac:dyDescent="0.65">
-      <c r="B1" s="40" t="s">
+      <c r="B1" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="40"/>
-      <c r="D1" s="40"/>
-      <c r="E1" s="40"/>
-      <c r="F1" s="40"/>
-      <c r="G1" s="40"/>
-      <c r="H1" s="40"/>
-      <c r="I1" s="40"/>
-      <c r="J1" s="40"/>
-      <c r="K1" s="21"/>
-      <c r="L1" s="21"/>
-      <c r="M1" s="21"/>
-      <c r="N1" s="21"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="20"/>
+      <c r="H1" s="20"/>
+      <c r="I1" s="20"/>
+      <c r="J1" s="20"/>
+      <c r="K1" s="20"/>
+      <c r="L1" s="20"/>
+      <c r="M1" s="20"/>
+      <c r="N1" s="20"/>
     </row>
     <row r="2" spans="1:20" ht="23.4" x14ac:dyDescent="0.3">
-      <c r="A2" s="35" t="s">
+      <c r="A2" s="32"/>
+    </row>
+    <row r="3" spans="1:20" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="A3" s="33"/>
+      <c r="C3" s="34"/>
+      <c r="D3" s="34"/>
+      <c r="E3" s="34"/>
+      <c r="F3" s="34"/>
+      <c r="G3" s="34"/>
+      <c r="H3" s="34"/>
+      <c r="I3" s="34"/>
+      <c r="J3" s="34"/>
+      <c r="K3" s="34"/>
+      <c r="L3" s="34"/>
+      <c r="M3" s="34"/>
+      <c r="N3" s="38"/>
+      <c r="P3" s="19"/>
+    </row>
+    <row r="4" spans="1:20" ht="23.4" x14ac:dyDescent="0.4">
+      <c r="A4" s="32" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" s="4">
+        <v>2022</v>
+      </c>
+      <c r="C4" s="35">
+        <v>2023</v>
+      </c>
+      <c r="D4" s="36"/>
+      <c r="E4" s="36"/>
+      <c r="F4" s="37"/>
+      <c r="G4" s="35">
+        <v>2024</v>
+      </c>
+      <c r="H4" s="36"/>
+      <c r="I4" s="36"/>
+      <c r="J4" s="37"/>
+      <c r="K4" s="39">
+        <v>2025</v>
+      </c>
+      <c r="L4" s="39"/>
+      <c r="M4" s="39"/>
+      <c r="S4" s="28"/>
+      <c r="T4" s="28"/>
+    </row>
+    <row r="5" spans="1:20" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="A5" s="33" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E5" s="4" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="3" spans="1:20" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="A3" s="36" t="s">
-        <v>16</v>
-      </c>
-      <c r="C3" s="41"/>
-      <c r="D3" s="41"/>
-      <c r="E3" s="41"/>
-      <c r="F3" s="41"/>
-      <c r="G3" s="41"/>
-      <c r="H3" s="41"/>
-      <c r="I3" s="41"/>
-      <c r="J3" s="41"/>
-      <c r="K3" s="41"/>
-      <c r="L3" s="41"/>
-      <c r="M3" s="41"/>
-      <c r="N3" s="41"/>
-      <c r="P3" s="20"/>
-    </row>
-    <row r="4" spans="1:20" ht="21" x14ac:dyDescent="0.4">
-      <c r="A4" s="26"/>
-      <c r="B4" s="20"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
-      <c r="H4" s="1"/>
-      <c r="I4" s="1"/>
-      <c r="J4" s="1"/>
-      <c r="K4" s="1"/>
-      <c r="L4" s="1"/>
-      <c r="M4" s="1"/>
-      <c r="N4" s="1"/>
-      <c r="P4" s="20"/>
-    </row>
-    <row r="5" spans="1:20" ht="21" x14ac:dyDescent="0.4">
-      <c r="B5" s="5">
-        <v>2022</v>
-      </c>
-      <c r="C5" s="37">
-        <v>2023</v>
-      </c>
-      <c r="D5" s="38"/>
-      <c r="E5" s="38"/>
-      <c r="F5" s="39"/>
-      <c r="G5" s="37">
-        <v>2024</v>
-      </c>
-      <c r="H5" s="38"/>
-      <c r="I5" s="38"/>
-      <c r="J5" s="39"/>
-      <c r="S5" s="31"/>
-      <c r="T5" s="31"/>
-    </row>
-    <row r="6" spans="1:20" ht="21" x14ac:dyDescent="0.3">
-      <c r="A6" s="20"/>
-      <c r="B6" s="5" t="s">
+      <c r="F5" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="I5" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="J5" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="K5" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="L5" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="M5" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="S5" s="6"/>
+      <c r="T5" s="6"/>
+    </row>
+    <row r="6" spans="1:20" ht="21" x14ac:dyDescent="0.4">
+      <c r="A6" s="40"/>
+      <c r="B6" s="9"/>
+      <c r="C6" s="9"/>
+      <c r="D6" s="9"/>
+      <c r="E6" s="9"/>
+      <c r="F6" s="9"/>
+      <c r="G6" s="9"/>
+      <c r="H6" s="9"/>
+      <c r="I6" s="9"/>
+      <c r="J6" s="9"/>
+      <c r="K6" s="9"/>
+      <c r="L6" s="9"/>
+      <c r="M6" s="9"/>
+      <c r="S6" s="12"/>
+      <c r="T6" s="12"/>
+    </row>
+    <row r="7" spans="1:20" ht="23.4" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A7" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="E6" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="F6" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="G6" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="H6" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="I6" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="J6" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="S6" s="7"/>
-      <c r="T6" s="7"/>
-    </row>
-    <row r="7" spans="1:20" ht="21" x14ac:dyDescent="0.4">
-      <c r="A7" s="3"/>
-      <c r="B7" s="10"/>
-      <c r="C7" s="10"/>
-      <c r="D7" s="10"/>
-      <c r="E7" s="10"/>
-      <c r="F7" s="10"/>
-      <c r="G7" s="10"/>
-      <c r="H7" s="10"/>
-      <c r="I7" s="10"/>
-      <c r="J7" s="10"/>
-      <c r="S7" s="13"/>
-      <c r="T7" s="13"/>
-    </row>
-    <row r="8" spans="1:20" ht="23.4" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A8" s="32" t="s">
-        <v>17</v>
-      </c>
-      <c r="B8" s="1"/>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+      <c r="S7" s="12"/>
+      <c r="T7" s="12"/>
+    </row>
+    <row r="8" spans="1:20" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A8" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="B8" s="11"/>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
-      <c r="S8" s="13"/>
-      <c r="T8" s="13"/>
+      <c r="S8" s="12"/>
+      <c r="T8" s="12"/>
     </row>
     <row r="9" spans="1:20" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A9" s="24" t="s">
-        <v>1</v>
-      </c>
-      <c r="B9" s="12"/>
-      <c r="C9" s="1"/>
+      <c r="A9" s="26" t="s">
+        <v>2</v>
+      </c>
+      <c r="B9" s="21"/>
+      <c r="C9" s="15"/>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
-      <c r="S9" s="13"/>
-      <c r="T9" s="13"/>
+      <c r="S9" s="12"/>
+      <c r="T9" s="12"/>
     </row>
     <row r="10" spans="1:20" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A10" s="28" t="s">
-        <v>2</v>
-      </c>
-      <c r="B10" s="22"/>
-      <c r="C10" s="16"/>
-      <c r="D10" s="1"/>
+      <c r="A10" s="22" t="s">
+        <v>3</v>
+      </c>
+      <c r="B10" s="10"/>
+      <c r="C10" s="11"/>
+      <c r="D10" s="11"/>
       <c r="E10" s="1"/>
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
-      <c r="S10" s="13"/>
-      <c r="T10" s="13"/>
-    </row>
-    <row r="11" spans="1:20" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A11" s="23" t="s">
-        <v>3</v>
-      </c>
-      <c r="B11" s="12"/>
-      <c r="C11" s="12"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
-      <c r="G11" s="1"/>
-      <c r="H11" s="1"/>
-      <c r="I11" s="1"/>
-      <c r="S11" s="13"/>
-      <c r="T11" s="13"/>
-    </row>
-    <row r="12" spans="1:20" s="4" customFormat="1" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A12" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="B12" s="11"/>
-      <c r="C12" s="12"/>
+      <c r="S10" s="12"/>
+      <c r="T10" s="12"/>
+    </row>
+    <row r="11" spans="1:20" s="3" customFormat="1" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A11" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11" s="10"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="11"/>
+      <c r="E11" s="11"/>
+      <c r="F11" s="11"/>
+      <c r="G11" s="11"/>
+      <c r="H11" s="10"/>
+      <c r="I11" s="10"/>
+      <c r="S11" s="12"/>
+      <c r="T11" s="12"/>
+    </row>
+    <row r="12" spans="1:20" ht="25.2" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A12" s="30" t="s">
+        <v>14</v>
+      </c>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
       <c r="D12" s="12"/>
-      <c r="E12" s="13"/>
-      <c r="G12" s="11"/>
-      <c r="H12" s="11"/>
-      <c r="I12" s="11"/>
-      <c r="S12" s="13"/>
-      <c r="T12" s="13"/>
-    </row>
-    <row r="13" spans="1:20" ht="25.2" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A13" s="33" t="s">
-        <v>18</v>
+      <c r="E12" s="12"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
+      <c r="I12" s="1"/>
+      <c r="S12" s="12"/>
+      <c r="T12" s="12"/>
+    </row>
+    <row r="13" spans="1:20" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A13" s="5" t="s">
+        <v>4</v>
       </c>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
-      <c r="D13" s="13"/>
-      <c r="E13" s="13"/>
-      <c r="G13" s="1"/>
-      <c r="H13" s="1"/>
+      <c r="D13" s="10"/>
+      <c r="E13" s="10"/>
+      <c r="F13" s="10"/>
+      <c r="G13" s="16"/>
+      <c r="H13" s="16"/>
       <c r="I13" s="1"/>
-      <c r="S13" s="13"/>
-      <c r="T13" s="13"/>
+      <c r="S13" s="12"/>
+      <c r="T13" s="12"/>
     </row>
     <row r="14" spans="1:20" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A14" s="6" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
-      <c r="D14" s="17"/>
-      <c r="E14" s="14"/>
-      <c r="G14" s="1"/>
-      <c r="H14" s="1"/>
-      <c r="I14" s="1"/>
-      <c r="S14" s="13"/>
-      <c r="T14" s="13"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="10"/>
+      <c r="F14" s="10"/>
+      <c r="G14" s="10"/>
+      <c r="H14" s="13"/>
+      <c r="I14" s="16"/>
+      <c r="S14" s="12"/>
+      <c r="T14" s="12"/>
     </row>
     <row r="15" spans="1:20" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A15" s="7" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
-      <c r="E15" s="29"/>
-      <c r="F15" s="14"/>
+      <c r="E15" s="12"/>
+      <c r="F15" s="10"/>
       <c r="G15" s="1"/>
-      <c r="H15" s="1"/>
-      <c r="I15" s="1"/>
-      <c r="S15" s="13"/>
-      <c r="T15" s="13"/>
-    </row>
-    <row r="16" spans="1:20" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A16" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="B16" s="1"/>
-      <c r="C16" s="1"/>
-      <c r="D16" s="1"/>
-      <c r="E16" s="13"/>
-      <c r="F16" s="14"/>
-      <c r="G16" s="1"/>
-      <c r="H16" s="1"/>
-      <c r="I16" s="1"/>
-      <c r="S16" s="13"/>
-      <c r="T16" s="13"/>
-    </row>
-    <row r="17" spans="1:20" ht="25.2" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A17" s="34" t="s">
-        <v>19</v>
-      </c>
-      <c r="B17" s="11"/>
-      <c r="C17" s="11"/>
-      <c r="D17" s="11"/>
-      <c r="E17" s="13"/>
-      <c r="F17" s="11"/>
-      <c r="G17" s="11"/>
-      <c r="H17" s="11"/>
-      <c r="I17" s="11"/>
-      <c r="S17" s="13"/>
-      <c r="T17" s="13"/>
+      <c r="H15" s="10"/>
+      <c r="I15" s="13"/>
+      <c r="S15" s="12"/>
+      <c r="T15" s="12"/>
+    </row>
+    <row r="16" spans="1:20" ht="25.2" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A16" s="31" t="s">
+        <v>15</v>
+      </c>
+      <c r="B16" s="10"/>
+      <c r="C16" s="10"/>
+      <c r="D16" s="10"/>
+      <c r="E16" s="12"/>
+      <c r="F16" s="10"/>
+      <c r="G16" s="10"/>
+      <c r="H16" s="10"/>
+      <c r="I16" s="10"/>
+      <c r="S16" s="12"/>
+      <c r="T16" s="12"/>
+    </row>
+    <row r="17" spans="1:20" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A17" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="12"/>
+      <c r="F17" s="1"/>
+      <c r="G17" s="12"/>
+      <c r="H17" s="12"/>
+      <c r="I17" s="24"/>
+      <c r="J17" s="14"/>
+      <c r="K17" s="14"/>
+      <c r="L17" s="14"/>
+      <c r="M17" s="14"/>
+      <c r="S17" s="12"/>
+      <c r="T17" s="12"/>
     </row>
     <row r="18" spans="1:20" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A18" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="B18" s="1"/>
-      <c r="C18" s="1"/>
-      <c r="D18" s="1"/>
-      <c r="E18" s="13"/>
-      <c r="F18" s="1"/>
-      <c r="G18" s="15"/>
-      <c r="H18" s="15"/>
-      <c r="I18" s="15"/>
-      <c r="J18" s="15"/>
-      <c r="S18" s="13"/>
-      <c r="T18" s="13"/>
-    </row>
-    <row r="19" spans="1:20" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A19" s="9" t="s">
+      <c r="A18" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="B19" s="11"/>
-      <c r="C19" s="11"/>
-      <c r="D19" s="11"/>
-      <c r="E19" s="13"/>
-      <c r="F19" s="11"/>
-      <c r="G19" s="30"/>
-      <c r="H19" s="13"/>
-      <c r="S19" s="13"/>
-      <c r="T19" s="13"/>
-    </row>
-    <row r="20" spans="1:20" s="4" customFormat="1" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A20" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="B20" s="11"/>
-      <c r="C20" s="11"/>
-      <c r="D20" s="11"/>
-      <c r="E20" s="13"/>
-      <c r="F20" s="11"/>
-      <c r="G20" s="13"/>
-      <c r="H20" s="13"/>
-      <c r="I20" s="30"/>
-      <c r="T20" s="13"/>
-    </row>
-    <row r="21" spans="1:20" s="4" customFormat="1" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A21" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="B21" s="11"/>
-      <c r="C21" s="11"/>
-      <c r="D21" s="11"/>
-      <c r="E21" s="13"/>
-      <c r="F21" s="11"/>
-      <c r="G21" s="13"/>
-      <c r="H21" s="13"/>
-      <c r="I21" s="25"/>
-      <c r="J21" s="15"/>
-      <c r="P21" s="13"/>
-      <c r="S21" s="13"/>
-    </row>
-    <row r="22" spans="1:20" s="4" customFormat="1" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A22" s="8" t="s">
+      <c r="B18" s="10"/>
+      <c r="C18" s="10"/>
+      <c r="D18" s="10"/>
+      <c r="E18" s="12"/>
+      <c r="F18" s="10"/>
+      <c r="G18" s="12"/>
+      <c r="H18" s="12"/>
+      <c r="I18" s="24"/>
+      <c r="J18" s="27"/>
+      <c r="K18" s="12"/>
+      <c r="S18" s="12"/>
+      <c r="T18" s="12"/>
+    </row>
+    <row r="19" spans="1:20" s="3" customFormat="1" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A19" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B19" s="10"/>
+      <c r="C19" s="10"/>
+      <c r="D19" s="10"/>
+      <c r="E19" s="12"/>
+      <c r="F19" s="10"/>
+      <c r="G19" s="12"/>
+      <c r="H19" s="12"/>
+      <c r="I19" s="24"/>
+      <c r="J19" s="12"/>
+      <c r="K19" s="12"/>
+      <c r="L19" s="27"/>
+      <c r="T19" s="12"/>
+    </row>
+    <row r="20" spans="1:20" s="3" customFormat="1" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A20" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B20" s="10"/>
+      <c r="C20" s="10"/>
+      <c r="D20" s="10"/>
+      <c r="E20" s="12"/>
+      <c r="F20" s="10"/>
+      <c r="G20" s="12"/>
+      <c r="H20" s="12"/>
+      <c r="I20" s="24"/>
+      <c r="J20" s="12"/>
+      <c r="K20" s="12"/>
+      <c r="L20" s="24"/>
+      <c r="M20" s="14"/>
+      <c r="P20" s="12"/>
+      <c r="S20" s="12"/>
+    </row>
+    <row r="21" spans="1:20" s="3" customFormat="1" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A21" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="B22" s="11"/>
-      <c r="C22" s="11"/>
-      <c r="D22" s="11"/>
-      <c r="E22" s="13"/>
-      <c r="F22" s="11"/>
-      <c r="G22" s="13"/>
-      <c r="H22" s="13"/>
-      <c r="I22" s="25"/>
-      <c r="J22" s="15"/>
-      <c r="P22" s="13"/>
-      <c r="S22" s="13"/>
-    </row>
-    <row r="24" spans="1:20" s="4" customFormat="1" ht="21" x14ac:dyDescent="0.4">
-      <c r="P24" s="13"/>
-    </row>
-    <row r="25" spans="1:20" s="4" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="P25" s="25"/>
+      <c r="B21" s="10"/>
+      <c r="C21" s="10"/>
+      <c r="D21" s="10"/>
+      <c r="E21" s="12"/>
+      <c r="F21" s="10"/>
+      <c r="G21" s="12"/>
+      <c r="H21" s="12"/>
+      <c r="I21" s="24"/>
+      <c r="J21" s="12"/>
+      <c r="K21" s="12"/>
+      <c r="L21" s="24"/>
+      <c r="M21" s="14"/>
+      <c r="P21" s="12"/>
+      <c r="S21" s="12"/>
+    </row>
+    <row r="23" spans="1:20" s="3" customFormat="1" ht="21" x14ac:dyDescent="0.4">
+      <c r="P23" s="12"/>
+    </row>
+    <row r="24" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="P24" s="24"/>
+    </row>
+    <row r="25" spans="1:20" ht="21" x14ac:dyDescent="0.4">
+      <c r="B25" s="1"/>
+      <c r="C25" s="1"/>
+      <c r="D25" s="1"/>
+      <c r="E25" s="12"/>
+      <c r="F25" s="1"/>
+      <c r="G25" s="1"/>
+      <c r="H25" s="1"/>
+      <c r="I25" s="1"/>
+      <c r="J25" s="1"/>
+      <c r="K25" s="1"/>
+      <c r="L25" s="1"/>
+      <c r="M25" s="2"/>
+      <c r="N25" s="18"/>
+      <c r="O25" s="12"/>
+      <c r="P25" s="19"/>
     </row>
     <row r="26" spans="1:20" ht="21" x14ac:dyDescent="0.4">
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
       <c r="D26" s="1"/>
-      <c r="E26" s="13"/>
+      <c r="E26" s="12"/>
       <c r="F26" s="1"/>
       <c r="G26" s="1"/>
       <c r="H26" s="1"/>
       <c r="I26" s="1"/>
-      <c r="J26" s="1"/>
+      <c r="J26" s="17"/>
       <c r="K26" s="1"/>
       <c r="L26" s="1"/>
-      <c r="M26" s="2"/>
-      <c r="N26" s="19"/>
-      <c r="O26" s="13"/>
-      <c r="P26" s="20"/>
+      <c r="M26" s="1"/>
+      <c r="N26" s="1"/>
+      <c r="O26" s="12"/>
     </row>
     <row r="27" spans="1:20" ht="21" x14ac:dyDescent="0.4">
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
       <c r="D27" s="1"/>
-      <c r="E27" s="13"/>
+      <c r="E27" s="12"/>
       <c r="F27" s="1"/>
       <c r="G27" s="1"/>
       <c r="H27" s="1"/>
       <c r="I27" s="1"/>
-      <c r="J27" s="18"/>
+      <c r="J27" s="1"/>
       <c r="K27" s="1"/>
       <c r="L27" s="1"/>
       <c r="M27" s="1"/>
       <c r="N27" s="1"/>
-      <c r="O27" s="13"/>
-    </row>
-    <row r="28" spans="1:20" ht="21" x14ac:dyDescent="0.4">
-      <c r="B28" s="1"/>
-      <c r="C28" s="1"/>
-      <c r="D28" s="1"/>
-      <c r="E28" s="13"/>
-      <c r="F28" s="1"/>
-      <c r="G28" s="1"/>
-      <c r="H28" s="1"/>
-      <c r="I28" s="1"/>
-      <c r="J28" s="1"/>
-      <c r="K28" s="1"/>
-      <c r="L28" s="1"/>
-      <c r="M28" s="1"/>
-      <c r="N28" s="1"/>
-      <c r="O28" s="1"/>
-    </row>
-    <row r="29" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="O29" s="20"/>
+      <c r="O27" s="1"/>
+    </row>
+    <row r="28" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="O28" s="19"/>
+    </row>
+    <row r="31" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A31" s="24"/>
+      <c r="B31" s="24"/>
+      <c r="C31" s="24"/>
+      <c r="D31" s="24"/>
+      <c r="E31" s="24"/>
     </row>
     <row r="32" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A32" s="25"/>
-      <c r="B32" s="25"/>
-      <c r="C32" s="25"/>
-      <c r="D32" s="25"/>
-      <c r="E32" s="25"/>
+      <c r="A32" s="24"/>
+      <c r="B32" s="24"/>
+      <c r="C32" s="24"/>
+      <c r="D32" s="24"/>
+      <c r="E32" s="24"/>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A33" s="25"/>
-      <c r="B33" s="25"/>
-      <c r="C33" s="25"/>
-      <c r="D33" s="25"/>
-      <c r="E33" s="25"/>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A34" s="25"/>
+      <c r="A33" s="24"/>
+      <c r="B33" s="24"/>
+      <c r="C33" s="24"/>
+      <c r="D33" s="24"/>
+      <c r="E33" s="24"/>
+    </row>
+    <row r="34" spans="1:5" ht="21" x14ac:dyDescent="0.3">
+      <c r="A34" s="24"/>
       <c r="B34" s="25"/>
       <c r="C34" s="25"/>
       <c r="D34" s="25"/>
-      <c r="E34" s="25"/>
+      <c r="E34" s="24"/>
     </row>
     <row r="35" spans="1:5" ht="21" x14ac:dyDescent="0.3">
-      <c r="A35" s="25"/>
-      <c r="B35" s="27"/>
-      <c r="C35" s="27"/>
-      <c r="D35" s="27"/>
-      <c r="E35" s="25"/>
-    </row>
-    <row r="36" spans="1:5" ht="21" x14ac:dyDescent="0.3">
-      <c r="A36" s="25"/>
-      <c r="B36" s="7"/>
-      <c r="C36" s="7"/>
-      <c r="D36" s="7"/>
-      <c r="E36" s="25"/>
+      <c r="A35" s="24"/>
+      <c r="B35" s="6"/>
+      <c r="C35" s="6"/>
+      <c r="D35" s="6"/>
+      <c r="E35" s="24"/>
+    </row>
+    <row r="36" spans="1:5" ht="21" x14ac:dyDescent="0.4">
+      <c r="A36" s="24"/>
+      <c r="B36" s="12"/>
+      <c r="C36" s="12"/>
+      <c r="D36" s="12"/>
+      <c r="E36" s="24"/>
     </row>
     <row r="37" spans="1:5" ht="21" x14ac:dyDescent="0.4">
-      <c r="A37" s="25"/>
-      <c r="B37" s="13"/>
-      <c r="C37" s="13"/>
-      <c r="D37" s="13"/>
-      <c r="E37" s="25"/>
+      <c r="A37" s="24"/>
+      <c r="B37" s="12"/>
+      <c r="C37" s="12"/>
+      <c r="D37" s="12"/>
+      <c r="E37" s="24"/>
     </row>
     <row r="38" spans="1:5" ht="21" x14ac:dyDescent="0.4">
-      <c r="A38" s="25"/>
-      <c r="B38" s="13"/>
-      <c r="C38" s="13"/>
-      <c r="D38" s="13"/>
-      <c r="E38" s="25"/>
+      <c r="A38" s="24"/>
+      <c r="B38" s="12"/>
+      <c r="C38" s="12"/>
+      <c r="D38" s="12"/>
+      <c r="E38" s="24"/>
     </row>
     <row r="39" spans="1:5" ht="21" x14ac:dyDescent="0.4">
-      <c r="A39" s="25"/>
-      <c r="B39" s="13"/>
-      <c r="C39" s="13"/>
-      <c r="D39" s="13"/>
-      <c r="E39" s="25"/>
+      <c r="A39" s="24"/>
+      <c r="B39" s="12"/>
+      <c r="C39" s="12"/>
+      <c r="D39" s="12"/>
+      <c r="E39" s="24"/>
     </row>
     <row r="40" spans="1:5" ht="21" x14ac:dyDescent="0.4">
-      <c r="A40" s="25"/>
-      <c r="B40" s="13"/>
-      <c r="C40" s="13"/>
-      <c r="D40" s="13"/>
-      <c r="E40" s="25"/>
+      <c r="A40" s="24"/>
+      <c r="B40" s="12"/>
+      <c r="C40" s="12"/>
+      <c r="D40" s="12"/>
+      <c r="E40" s="24"/>
     </row>
     <row r="41" spans="1:5" ht="21" x14ac:dyDescent="0.4">
-      <c r="A41" s="25"/>
-      <c r="B41" s="13"/>
-      <c r="C41" s="13"/>
-      <c r="D41" s="13"/>
-      <c r="E41" s="25"/>
+      <c r="A41" s="24"/>
+      <c r="B41" s="12"/>
+      <c r="C41" s="12"/>
+      <c r="D41" s="12"/>
+      <c r="E41" s="24"/>
     </row>
     <row r="42" spans="1:5" ht="21" x14ac:dyDescent="0.4">
-      <c r="A42" s="25"/>
-      <c r="B42" s="13"/>
-      <c r="C42" s="13"/>
-      <c r="D42" s="13"/>
-      <c r="E42" s="25"/>
-    </row>
-    <row r="43" spans="1:5" ht="21" x14ac:dyDescent="0.4">
-      <c r="A43" s="25"/>
-      <c r="B43" s="13"/>
-      <c r="C43" s="13"/>
-      <c r="D43" s="13"/>
-      <c r="E43" s="25"/>
+      <c r="A42" s="24"/>
+      <c r="B42" s="12"/>
+      <c r="C42" s="12"/>
+      <c r="D42" s="12"/>
+      <c r="E42" s="24"/>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A43" s="24"/>
+      <c r="B43" s="24"/>
+      <c r="C43" s="24"/>
+      <c r="D43" s="24"/>
+      <c r="E43" s="24"/>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A44" s="25"/>
-      <c r="B44" s="25"/>
-      <c r="C44" s="25"/>
-      <c r="D44" s="25"/>
-      <c r="E44" s="25"/>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A45" s="25"/>
-      <c r="B45" s="25"/>
-      <c r="C45" s="25"/>
-      <c r="D45" s="25"/>
-      <c r="E45" s="25"/>
+      <c r="A44" s="24"/>
+      <c r="B44" s="24"/>
+      <c r="C44" s="24"/>
+      <c r="D44" s="24"/>
+      <c r="E44" s="24"/>
     </row>
   </sheetData>
   <mergeCells count="6">
-    <mergeCell ref="K3:N3"/>
-    <mergeCell ref="C5:F5"/>
-    <mergeCell ref="G5:J5"/>
-    <mergeCell ref="B1:J1"/>
+    <mergeCell ref="C4:F4"/>
+    <mergeCell ref="G4:J4"/>
     <mergeCell ref="C3:F3"/>
     <mergeCell ref="G3:J3"/>
+    <mergeCell ref="K3:M3"/>
+    <mergeCell ref="K4:M4"/>
   </mergeCells>
-  <phoneticPr fontId="5" type="noConversion"/>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>